<commit_message>
Refactoring of existing tests (where required) and made a start on Give Feedback tests
</commit_message>
<xml_diff>
--- a/Data Files/Search_CAT_ID_Data.xlsx
+++ b/Data Files/Search_CAT_ID_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44029EF-7547-4747-9AC5-21F6E077AC93}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89A85C5-5EC9-42C1-9C1C-6D5107FED4FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4530" yWindow="2415" windowWidth="21600" windowHeight="11145" xr2:uid="{56648964-8086-4401-B8BD-AFCFF037A6DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{56648964-8086-4401-B8BD-AFCFF037A6DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Gosport</t>
   </si>
@@ -133,27 +133,6 @@
   </si>
   <si>
     <t>Searches on CAT ID - Verified Retuned Data</t>
-  </si>
-  <si>
-    <t>Fireplaces/Stoves</t>
-  </si>
-  <si>
-    <t>Mr Daniel Moon</t>
-  </si>
-  <si>
-    <t>Southborough, Tunbridge Wells, Kent</t>
-  </si>
-  <si>
-    <t>Kent</t>
-  </si>
-  <si>
-    <t>Fireplaces/Stoves in Kent</t>
-  </si>
-  <si>
-    <t>Location not found</t>
-  </si>
-  <si>
-    <t>Searches on CAT ID - Location Not Found</t>
   </si>
   <si>
     <t>error_Messages_Returned</t>
@@ -163,7 +142,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,25 +150,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -204,13 +171,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D56B88-33E9-468B-853E-05EE5D8A6600}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -566,7 +531,7 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="I1" t="s">
         <v>32</v>
@@ -700,32 +665,6 @@
       </c>
       <c r="I6" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="1">
-        <v>373735</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Web Office - Initial Stuff, Searching on trade/name/Phone from WO Search H
</commit_message>
<xml_diff>
--- a/Data Files/Search_CAT_ID_Data.xlsx
+++ b/Data Files/Search_CAT_ID_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidho\Katalon Studio\Start\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89A85C5-5EC9-42C1-9C1C-6D5107FED4FD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E46BF3-E26E-422A-887C-5B72CBEF43EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{56648964-8086-4401-B8BD-AFCFF037A6DE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{56648964-8086-4401-B8BD-AFCFF037A6DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>Gosport</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Andrew Whitaker</t>
   </si>
   <si>
-    <t>Dan Hunt</t>
-  </si>
-  <si>
     <t>tradeClassification</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>Retford, Nottinghamshire</t>
   </si>
   <si>
-    <t>Littlehampton, West Sussex</t>
-  </si>
-  <si>
     <t>comments</t>
   </si>
   <si>
@@ -136,19 +130,34 @@
   </si>
   <si>
     <t>error_Messages_Returned</t>
+  </si>
+  <si>
+    <t>David Clarke</t>
+  </si>
+  <si>
+    <t>Rustington</t>
+  </si>
+  <si>
+    <t>Rustington, West Sussex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,11 +180,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,36 +503,36 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.265625" customWidth="1"/>
-    <col min="2" max="2" width="28.73046875" customWidth="1"/>
-    <col min="3" max="3" width="36.3984375" customWidth="1"/>
-    <col min="4" max="4" width="27.3984375" customWidth="1"/>
-    <col min="5" max="5" width="18.1328125" customWidth="1"/>
-    <col min="6" max="6" width="21.1328125" customWidth="1"/>
-    <col min="7" max="8" width="35.86328125" customWidth="1"/>
-    <col min="9" max="9" width="44.59765625" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="8" width="35.85546875" customWidth="1"/>
+    <col min="9" max="9" width="44.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
         <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>29</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -531,13 +541,13 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>218020</v>
       </c>
@@ -551,19 +561,19 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>402921</v>
       </c>
@@ -571,25 +581,25 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
       </c>
       <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>308682</v>
       </c>
@@ -603,45 +613,45 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>230761</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="1">
-        <v>81557</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>381198</v>
       </c>
@@ -655,16 +665,16 @@
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>